<commit_message>
Commit after data manipulation and before figures
</commit_message>
<xml_diff>
--- a/Data/Mill_Pop.xlsx
+++ b/Data/Mill_Pop.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sameernair-desai/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timodaehler/Desktop/COVID19-DOMINANCE/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23ADC899-057E-4144-B008-48BB5F98ED41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA484055-EA88-2642-98A9-ED9F3B5EAD6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12940" yWindow="1980" windowWidth="28040" windowHeight="16820" xr2:uid="{6DECCBCC-4377-A34E-A6DD-BAC1FBC13F3E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{BFBFA1AB-A43A-2244-AEF0-91A8455F8FF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,76 +33,136 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+  <si>
+    <t>Peru</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Panama</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>Bahrain</t>
+  </si>
+  <si>
+    <t>Saudi Arabia</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Dominican Republic</t>
+  </si>
+  <si>
+    <t>Oman</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>Azerbaijan</t>
+  </si>
+  <si>
+    <t>Czechia</t>
+  </si>
+  <si>
+    <t>Ukraine</t>
+  </si>
+  <si>
+    <t>Kazakhstan</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
   <si>
     <t>COUNTRY</t>
   </si>
   <si>
-    <t>Population (Millions)</t>
-  </si>
-  <si>
-    <t>Austria</t>
-  </si>
-  <si>
-    <t>Belgium</t>
-  </si>
-  <si>
-    <t>Cyprus</t>
-  </si>
-  <si>
-    <t>Estonia</t>
-  </si>
-  <si>
-    <t>Finland</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>Germany</t>
-  </si>
-  <si>
-    <t>Greece</t>
-  </si>
-  <si>
-    <t>Ireland</t>
-  </si>
-  <si>
-    <t>Italy</t>
-  </si>
-  <si>
-    <t>Latvia</t>
-  </si>
-  <si>
-    <t>Lithuania</t>
-  </si>
-  <si>
-    <t>Netherlands</t>
-  </si>
-  <si>
-    <t>Portugal</t>
-  </si>
-  <si>
-    <t>Slovakia</t>
-  </si>
-  <si>
-    <t>Slovenia</t>
-  </si>
-  <si>
-    <t>Spain</t>
+    <t>PopMil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF696969"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -125,8 +185,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,163 +502,751 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01AB597D-720C-E14B-9AF0-A8A538A6F481}">
-  <dimension ref="A1:B18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAE3298F-E724-CB4C-A64B-7344D0A5ECFA}">
+  <dimension ref="A1:B148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>8.85</v>
+        <v>16</v>
+      </c>
+      <c r="B2" s="2">
+        <v>44.49</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>11.42</v>
+        <v>20</v>
+      </c>
+      <c r="B3" s="2">
+        <v>9.94</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>1.19</v>
+        <v>9</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.57</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>1.32</v>
+        <v>2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>209.47</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>5.52</v>
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
+        <v>18.73</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>66.989999999999995</v>
+        <v>31</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1392.73</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>82.93</v>
+        <v>5</v>
+      </c>
+      <c r="B8" s="2">
+        <v>49.65</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>10.73</v>
+        <v>21</v>
+      </c>
+      <c r="B9" s="2">
+        <v>10.63</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>4.8499999999999996</v>
+        <v>13</v>
+      </c>
+      <c r="B10" s="2">
+        <v>10.63</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>60.43</v>
+        <v>18</v>
+      </c>
+      <c r="B11" s="2">
+        <v>98.42</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>1.93</v>
+        <v>28</v>
+      </c>
+      <c r="B12" s="2">
+        <v>29.77</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <v>2.79</v>
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>9.77</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>17.23</v>
+        <v>24</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1352.62</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
-        <v>10.28</v>
+        <v>26</v>
+      </c>
+      <c r="B15" s="2">
+        <v>267.66000000000003</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16">
-        <v>5.45</v>
+        <v>23</v>
+      </c>
+      <c r="B16" s="2">
+        <v>18.28</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17">
-        <v>2.0699999999999998</v>
+        <v>30</v>
+      </c>
+      <c r="B17" s="2">
+        <v>31.53</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18">
-        <v>46.72</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B18" s="2">
+        <v>126.19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="2">
+        <v>195.87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="2">
+        <v>4.83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="2">
+        <v>4.18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="2">
+        <v>31.99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="2">
+        <v>106.65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="2">
+        <v>37.979999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2">
+        <v>19.47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="2">
+        <v>144.47999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="2">
+        <v>33.700000000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="2">
+        <v>57.78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="2">
+        <v>21.67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="2">
+        <v>69.430000000000007</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="2">
+        <v>82.32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="2">
+        <v>44.62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="2">
+        <v>9.6300000000000008</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="2">
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+    </row>
+    <row r="52" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+    </row>
+    <row r="54" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+    </row>
+    <row r="55" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+    </row>
+    <row r="56" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+    </row>
+    <row r="58" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+    </row>
+    <row r="59" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+    </row>
+    <row r="60" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+    </row>
+    <row r="61" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+    </row>
+    <row r="63" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+    </row>
+    <row r="65" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+    </row>
+    <row r="69" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+    </row>
+    <row r="70" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+    </row>
+    <row r="71" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+    </row>
+    <row r="72" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+    </row>
+    <row r="73" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+    </row>
+    <row r="75" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+    </row>
+    <row r="76" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+    </row>
+    <row r="77" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+    </row>
+    <row r="78" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+    </row>
+    <row r="79" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+    </row>
+    <row r="80" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+    </row>
+    <row r="81" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+    </row>
+    <row r="82" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+    </row>
+    <row r="83" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+    </row>
+    <row r="84" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+    </row>
+    <row r="85" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+    </row>
+    <row r="86" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+    </row>
+    <row r="87" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+    </row>
+    <row r="88" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+    </row>
+    <row r="89" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+    </row>
+    <row r="90" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+    </row>
+    <row r="91" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+    </row>
+    <row r="92" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+    </row>
+    <row r="93" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+    </row>
+    <row r="94" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+    </row>
+    <row r="95" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+    </row>
+    <row r="96" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+    </row>
+    <row r="97" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+    </row>
+    <row r="98" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+    </row>
+    <row r="99" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+    </row>
+    <row r="100" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+    </row>
+    <row r="101" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+    </row>
+    <row r="102" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+    </row>
+    <row r="103" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+    </row>
+    <row r="104" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+    </row>
+    <row r="105" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+    </row>
+    <row r="106" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+    </row>
+    <row r="107" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+    </row>
+    <row r="108" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+    </row>
+    <row r="109" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+    </row>
+    <row r="110" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+    </row>
+    <row r="111" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+    </row>
+    <row r="112" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+    </row>
+    <row r="113" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+    </row>
+    <row r="114" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+    </row>
+    <row r="115" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
+    </row>
+    <row r="116" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+    </row>
+    <row r="117" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A117" s="1"/>
+      <c r="B117" s="1"/>
+    </row>
+    <row r="118" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
+    </row>
+    <row r="119" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
+    </row>
+    <row r="120" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
+    </row>
+    <row r="121" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A121" s="1"/>
+      <c r="B121" s="1"/>
+    </row>
+    <row r="122" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A122" s="1"/>
+      <c r="B122" s="1"/>
+    </row>
+    <row r="123" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A123" s="1"/>
+      <c r="B123" s="1"/>
+    </row>
+    <row r="124" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
+    </row>
+    <row r="125" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A125" s="1"/>
+      <c r="B125" s="1"/>
+    </row>
+    <row r="126" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A126" s="1"/>
+      <c r="B126" s="1"/>
+    </row>
+    <row r="127" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A127" s="1"/>
+      <c r="B127" s="1"/>
+    </row>
+    <row r="128" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A128" s="1"/>
+      <c r="B128" s="1"/>
+    </row>
+    <row r="129" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A129" s="1"/>
+      <c r="B129" s="1"/>
+    </row>
+    <row r="130" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A130" s="1"/>
+      <c r="B130" s="1"/>
+    </row>
+    <row r="131" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A131" s="1"/>
+      <c r="B131" s="1"/>
+    </row>
+    <row r="132" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A132" s="1"/>
+      <c r="B132" s="1"/>
+    </row>
+    <row r="133" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A133" s="1"/>
+      <c r="B133" s="1"/>
+    </row>
+    <row r="134" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A134" s="1"/>
+      <c r="B134" s="1"/>
+    </row>
+    <row r="135" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A135" s="1"/>
+      <c r="B135" s="1"/>
+    </row>
+    <row r="136" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A136" s="1"/>
+      <c r="B136" s="1"/>
+    </row>
+    <row r="137" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A137" s="1"/>
+      <c r="B137" s="1"/>
+    </row>
+    <row r="138" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A138" s="1"/>
+      <c r="B138" s="1"/>
+    </row>
+    <row r="139" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A139" s="1"/>
+      <c r="B139" s="1"/>
+    </row>
+    <row r="140" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A140" s="1"/>
+      <c r="B140" s="1"/>
+    </row>
+    <row r="141" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A141" s="1"/>
+      <c r="B141" s="1"/>
+    </row>
+    <row r="142" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A142" s="1"/>
+      <c r="B142" s="1"/>
+    </row>
+    <row r="143" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A143" s="1"/>
+      <c r="B143" s="1"/>
+    </row>
+    <row r="144" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A144" s="1"/>
+      <c r="B144" s="1"/>
+    </row>
+    <row r="145" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A145" s="1"/>
+      <c r="B145" s="1"/>
+    </row>
+    <row r="146" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A146" s="1"/>
+      <c r="B146" s="1"/>
+    </row>
+    <row r="147" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A147" s="1"/>
+      <c r="B147" s="1"/>
+    </row>
+    <row r="148" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A148" s="1"/>
+      <c r="B148" s="1"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B35">
+    <sortCondition ref="A2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>